<commit_message>
clean up + updated trainer structure (althought not pushed)
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alirachidi/Documents/Sonavi_Labs/classification_algorithm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41313E63-7DF1-B54E-8868-3034080D98F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4427419-9730-EA46-A191-94B65B72492F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="19140" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="for_loop_v1" sheetId="1" r:id="rId1"/>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1017,7 +1017,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1911,10 +1911,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -2305,7 +2305,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2514,7 +2514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2723,10 +2723,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>

</xml_diff>